<commit_message>
feat(translation): variable translation for hi,ml and te
</commit_message>
<xml_diff>
--- a/utils/localisation_script/excel_to_json/gu/t.xlsx
+++ b/utils/localisation_script/excel_to_json/gu/t.xlsx
@@ -5,17 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/umair.manzoor/Projects/Open-Speech-EkStep/crowdsource-dataplatform/utils/localisation_script/excel_to_json/gu/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sreejithv/TW/projects/ekStep/crowdsource-dataplatform/utils/localisation_script/excel_to_json/gu/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EBC39D3-D867-814D-83CC-35BF7920CC9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3127BF58-D429-0441-B4E0-504BBB25D10E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="20500" windowHeight="7760" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Delta" sheetId="7" r:id="rId1"/>
     <sheet name="Delta 2" sheetId="8" r:id="rId2"/>
-    <sheet name="Sheet10" sheetId="9" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
@@ -7691,19 +7690,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>